<commit_message>
Se actualiza cuadro de control con los últimos avances
</commit_message>
<xml_diff>
--- a/proy_tanques_2.0/cuadro-control-proyecto-tanques2.0.xlsx
+++ b/proy_tanques_2.0/cuadro-control-proyecto-tanques2.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Francisco\personal_Projects_WS\proy_tanques_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05F8BB8-E5E4-46AC-9583-49A42DA70550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5401999C-6AC1-45FF-A668-3478665637F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1065,7 +1065,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1077,7 +1077,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,7 +1416,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.125</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1425,7 +1425,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.875</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31179,10 +31179,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:DG1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="M11" sqref="M11"/>
+      <selection pane="topRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -32590,12 +32590,14 @@
         <v>36</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="41"/>
-      <c r="N11" s="42" t="str">
+        <v>22</v>
+      </c>
+      <c r="M11" s="41">
+        <v>45094</v>
+      </c>
+      <c r="N11" s="42">
         <f t="shared" si="2"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="P11" s="43" t="str">
         <f t="shared" ref="P11:DA11" si="8">IF(AND(P$8&gt;=$I11,P$8&lt;=$J11),"x","")</f>
@@ -32963,7 +32965,7 @@
       </c>
       <c r="DD11" s="34">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:111" ht="14.25" customHeight="1">
@@ -40932,7 +40934,7 @@
       </c>
       <c r="C3" s="57">
         <f ca="1">TODAY()</f>
-        <v>45081</v>
+        <v>45094</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="14.25" customHeight="1">
@@ -40950,7 +40952,7 @@
       </c>
       <c r="C5" s="58">
         <f ca="1">IF(Proyecto!D4="","",C3-Proyecto!D4)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="14.25" customHeight="1">
@@ -40959,7 +40961,7 @@
       </c>
       <c r="C6" s="58">
         <f ca="1">IF(Proyecto!D4="","",C4-C5)</f>
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="N6" s="59" t="s">
         <v>30</v>
@@ -40972,7 +40974,7 @@
       </c>
       <c r="R6" s="61">
         <f>IF(COUNTA(Proyecto!$L$9:$L$28)=0,NA(),COUNTIF(Proyecto!$L$9:$L$28,Reportes!Q6)/COUNTA(Proyecto!$L$9:$L$28))</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="14.25" customHeight="1">
@@ -41038,7 +41040,7 @@
       </c>
       <c r="R9" s="61">
         <f>IF(COUNTA(Proyecto!$L$9:$L$28)=0,NA(),COUNTIF(Proyecto!$L$9:$L$28,Reportes!Q9)/COUNTA(Proyecto!$L$9:$L$28))</f>
-        <v>0.875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="14.25" customHeight="1">
@@ -41285,7 +41287,7 @@
       </c>
       <c r="G25" s="71">
         <f>SUM(Proyecto!DD9:DD28)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I25" s="68"/>
       <c r="J25" s="68"/>

</xml_diff>